<commit_message>
Update mockup with endpoints
</commit_message>
<xml_diff>
--- a/documentation/Mockup.xlsx
+++ b/documentation/Mockup.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="56">
   <si>
     <t>Elementos</t>
   </si>
@@ -178,6 +178,15 @@
   </si>
   <si>
     <t>Borrar formulario</t>
+  </si>
+  <si>
+    <t>Respuestas</t>
+  </si>
+  <si>
+    <t>500 la tendrán todos</t>
+  </si>
+  <si>
+    <t>Comentarios</t>
   </si>
 </sst>
 </file>
@@ -347,7 +356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -363,6 +372,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -385,10 +398,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -24576,132 +24595,132 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="39" spans="3:38" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="7" t="s">
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H39" s="7"/>
-      <c r="I39" s="7"/>
-      <c r="J39" s="7"/>
-      <c r="K39" s="7"/>
-      <c r="L39" s="7"/>
-      <c r="M39" s="7"/>
-      <c r="N39" s="7"/>
-      <c r="O39" s="7"/>
-      <c r="P39" s="7"/>
-      <c r="Q39" s="7"/>
-      <c r="R39" s="7"/>
-      <c r="S39" s="7"/>
-      <c r="T39" s="7"/>
-      <c r="U39" s="6" t="s">
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="9"/>
+      <c r="K39" s="9"/>
+      <c r="L39" s="9"/>
+      <c r="M39" s="9"/>
+      <c r="N39" s="9"/>
+      <c r="O39" s="9"/>
+      <c r="P39" s="9"/>
+      <c r="Q39" s="9"/>
+      <c r="R39" s="9"/>
+      <c r="S39" s="9"/>
+      <c r="T39" s="9"/>
+      <c r="U39" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="V39" s="6"/>
-      <c r="W39" s="6"/>
-      <c r="X39" s="6"/>
-      <c r="Y39" s="6"/>
-      <c r="Z39" s="6" t="s">
+      <c r="V39" s="8"/>
+      <c r="W39" s="8"/>
+      <c r="X39" s="8"/>
+      <c r="Y39" s="8"/>
+      <c r="Z39" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="AA39" s="6"/>
-      <c r="AB39" s="6"/>
-      <c r="AC39" s="6"/>
-      <c r="AD39" s="6"/>
-      <c r="AE39" s="6"/>
-      <c r="AF39" s="6" t="s">
+      <c r="AA39" s="8"/>
+      <c r="AB39" s="8"/>
+      <c r="AC39" s="8"/>
+      <c r="AD39" s="8"/>
+      <c r="AE39" s="8"/>
+      <c r="AF39" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="AG39" s="6"/>
-      <c r="AH39" s="6"/>
-      <c r="AI39" s="6"/>
-      <c r="AJ39" s="6"/>
-      <c r="AK39" s="6"/>
-      <c r="AL39" s="6"/>
+      <c r="AG39" s="8"/>
+      <c r="AH39" s="8"/>
+      <c r="AI39" s="8"/>
+      <c r="AJ39" s="8"/>
+      <c r="AK39" s="8"/>
+      <c r="AL39" s="8"/>
     </row>
     <row r="40" spans="3:38" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="7" t="s">
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="H40" s="7"/>
-      <c r="I40" s="7"/>
-      <c r="J40" s="7"/>
-      <c r="K40" s="7"/>
-      <c r="L40" s="7"/>
-      <c r="M40" s="7"/>
-      <c r="N40" s="7"/>
-      <c r="O40" s="7"/>
-      <c r="P40" s="7"/>
-      <c r="Q40" s="7"/>
-      <c r="R40" s="7"/>
-      <c r="S40" s="7"/>
-      <c r="T40" s="7"/>
-      <c r="U40" s="6"/>
-      <c r="V40" s="6"/>
-      <c r="W40" s="6"/>
-      <c r="X40" s="6"/>
-      <c r="Y40" s="6"/>
-      <c r="Z40" s="6"/>
-      <c r="AA40" s="6"/>
-      <c r="AB40" s="6"/>
-      <c r="AC40" s="6"/>
-      <c r="AD40" s="6"/>
-      <c r="AE40" s="6"/>
-      <c r="AF40" s="6"/>
-      <c r="AG40" s="6"/>
-      <c r="AH40" s="6"/>
-      <c r="AI40" s="6"/>
-      <c r="AJ40" s="6"/>
-      <c r="AK40" s="6"/>
-      <c r="AL40" s="6"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="9"/>
+      <c r="K40" s="9"/>
+      <c r="L40" s="9"/>
+      <c r="M40" s="9"/>
+      <c r="N40" s="9"/>
+      <c r="O40" s="9"/>
+      <c r="P40" s="9"/>
+      <c r="Q40" s="9"/>
+      <c r="R40" s="9"/>
+      <c r="S40" s="9"/>
+      <c r="T40" s="9"/>
+      <c r="U40" s="8"/>
+      <c r="V40" s="8"/>
+      <c r="W40" s="8"/>
+      <c r="X40" s="8"/>
+      <c r="Y40" s="8"/>
+      <c r="Z40" s="8"/>
+      <c r="AA40" s="8"/>
+      <c r="AB40" s="8"/>
+      <c r="AC40" s="8"/>
+      <c r="AD40" s="8"/>
+      <c r="AE40" s="8"/>
+      <c r="AF40" s="8"/>
+      <c r="AG40" s="8"/>
+      <c r="AH40" s="8"/>
+      <c r="AI40" s="8"/>
+      <c r="AJ40" s="8"/>
+      <c r="AK40" s="8"/>
+      <c r="AL40" s="8"/>
     </row>
     <row r="41" spans="3:38" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="7" t="s">
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="H41" s="7"/>
-      <c r="I41" s="7"/>
-      <c r="J41" s="7"/>
-      <c r="K41" s="7"/>
-      <c r="L41" s="7"/>
-      <c r="M41" s="7"/>
-      <c r="N41" s="7"/>
-      <c r="O41" s="7"/>
-      <c r="P41" s="7"/>
-      <c r="Q41" s="7"/>
-      <c r="R41" s="7"/>
-      <c r="S41" s="7"/>
-      <c r="T41" s="7"/>
-      <c r="U41" s="6"/>
-      <c r="V41" s="6"/>
-      <c r="W41" s="6"/>
-      <c r="X41" s="6"/>
-      <c r="Y41" s="6"/>
-      <c r="Z41" s="6"/>
-      <c r="AA41" s="6"/>
-      <c r="AB41" s="6"/>
-      <c r="AC41" s="6"/>
-      <c r="AD41" s="6"/>
-      <c r="AE41" s="6"/>
-      <c r="AF41" s="6"/>
-      <c r="AG41" s="6"/>
-      <c r="AH41" s="6"/>
-      <c r="AI41" s="6"/>
-      <c r="AJ41" s="6"/>
-      <c r="AK41" s="6"/>
-      <c r="AL41" s="6"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
+      <c r="J41" s="9"/>
+      <c r="K41" s="9"/>
+      <c r="L41" s="9"/>
+      <c r="M41" s="9"/>
+      <c r="N41" s="9"/>
+      <c r="O41" s="9"/>
+      <c r="P41" s="9"/>
+      <c r="Q41" s="9"/>
+      <c r="R41" s="9"/>
+      <c r="S41" s="9"/>
+      <c r="T41" s="9"/>
+      <c r="U41" s="8"/>
+      <c r="V41" s="8"/>
+      <c r="W41" s="8"/>
+      <c r="X41" s="8"/>
+      <c r="Y41" s="8"/>
+      <c r="Z41" s="8"/>
+      <c r="AA41" s="8"/>
+      <c r="AB41" s="8"/>
+      <c r="AC41" s="8"/>
+      <c r="AD41" s="8"/>
+      <c r="AE41" s="8"/>
+      <c r="AF41" s="8"/>
+      <c r="AG41" s="8"/>
+      <c r="AH41" s="8"/>
+      <c r="AI41" s="8"/>
+      <c r="AJ41" s="8"/>
+      <c r="AK41" s="8"/>
+      <c r="AL41" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -24730,53 +24749,53 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="35" spans="3:17" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C35" s="9" t="s">
+      <c r="C35" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="10" t="s">
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="11"/>
-      <c r="K35" s="12"/>
-      <c r="L35" s="6" t="s">
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="14"/>
+      <c r="L35" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="M35" s="6"/>
-      <c r="N35" s="6"/>
-      <c r="O35" s="6"/>
-      <c r="P35" s="6"/>
-      <c r="Q35" s="6"/>
+      <c r="M35" s="8"/>
+      <c r="N35" s="8"/>
+      <c r="O35" s="8"/>
+      <c r="P35" s="8"/>
+      <c r="Q35" s="8"/>
     </row>
     <row r="36" spans="3:17" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="10" t="s">
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="11"/>
-      <c r="K36" s="12"/>
-      <c r="L36" s="6"/>
-      <c r="M36" s="6"/>
-      <c r="N36" s="6"/>
-      <c r="O36" s="6"/>
-      <c r="P36" s="6"/>
-      <c r="Q36" s="6"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="14"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8"/>
+      <c r="N36" s="8"/>
+      <c r="O36" s="8"/>
+      <c r="P36" s="8"/>
+      <c r="Q36" s="8"/>
     </row>
     <row r="72" spans="3:31" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C72" s="9" t="s">
+      <c r="C72" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D72" s="9"/>
-      <c r="E72" s="9"/>
+      <c r="D72" s="11"/>
+      <c r="E72" s="11"/>
       <c r="F72" s="1" t="s">
         <v>9</v>
       </c>
@@ -24784,38 +24803,38 @@
       <c r="H72" s="2"/>
       <c r="I72" s="2"/>
       <c r="J72" s="3"/>
-      <c r="K72" s="7" t="s">
+      <c r="K72" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L72" s="7"/>
-      <c r="M72" s="7"/>
-      <c r="N72" s="7"/>
-      <c r="O72" s="7"/>
-      <c r="P72" s="7"/>
-      <c r="Q72" s="7"/>
-      <c r="R72" s="6" t="s">
+      <c r="L72" s="9"/>
+      <c r="M72" s="9"/>
+      <c r="N72" s="9"/>
+      <c r="O72" s="9"/>
+      <c r="P72" s="9"/>
+      <c r="Q72" s="9"/>
+      <c r="R72" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="S72" s="6"/>
-      <c r="T72" s="6"/>
-      <c r="U72" s="6"/>
-      <c r="V72" s="6"/>
-      <c r="W72" s="6"/>
-      <c r="X72" s="6"/>
-      <c r="Y72" s="7" t="s">
+      <c r="S72" s="8"/>
+      <c r="T72" s="8"/>
+      <c r="U72" s="8"/>
+      <c r="V72" s="8"/>
+      <c r="W72" s="8"/>
+      <c r="X72" s="8"/>
+      <c r="Y72" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="Z72" s="7"/>
-      <c r="AA72" s="7"/>
-      <c r="AB72" s="7"/>
-      <c r="AC72" s="7"/>
-      <c r="AD72" s="7"/>
-      <c r="AE72" s="7"/>
+      <c r="Z72" s="9"/>
+      <c r="AA72" s="9"/>
+      <c r="AB72" s="9"/>
+      <c r="AC72" s="9"/>
+      <c r="AD72" s="9"/>
+      <c r="AE72" s="9"/>
     </row>
     <row r="73" spans="3:31" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="C73" s="9"/>
-      <c r="D73" s="9"/>
-      <c r="E73" s="9"/>
+      <c r="C73" s="11"/>
+      <c r="D73" s="11"/>
+      <c r="E73" s="11"/>
       <c r="F73" s="1" t="s">
         <v>14</v>
       </c>
@@ -24823,53 +24842,53 @@
       <c r="H73" s="4"/>
       <c r="I73" s="4"/>
       <c r="J73" s="5"/>
-      <c r="K73" s="7" t="s">
+      <c r="K73" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L73" s="7"/>
-      <c r="M73" s="7"/>
-      <c r="N73" s="7"/>
-      <c r="O73" s="7"/>
-      <c r="P73" s="7"/>
-      <c r="Q73" s="7"/>
-      <c r="R73" s="6"/>
-      <c r="S73" s="6"/>
-      <c r="T73" s="6"/>
-      <c r="U73" s="6"/>
-      <c r="V73" s="6"/>
-      <c r="W73" s="6"/>
-      <c r="X73" s="6"/>
-      <c r="Y73" s="7" t="s">
+      <c r="L73" s="9"/>
+      <c r="M73" s="9"/>
+      <c r="N73" s="9"/>
+      <c r="O73" s="9"/>
+      <c r="P73" s="9"/>
+      <c r="Q73" s="9"/>
+      <c r="R73" s="8"/>
+      <c r="S73" s="8"/>
+      <c r="T73" s="8"/>
+      <c r="U73" s="8"/>
+      <c r="V73" s="8"/>
+      <c r="W73" s="8"/>
+      <c r="X73" s="8"/>
+      <c r="Y73" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="Z73" s="7"/>
-      <c r="AA73" s="7"/>
-      <c r="AB73" s="7"/>
-      <c r="AC73" s="7"/>
-      <c r="AD73" s="7"/>
-      <c r="AE73" s="7"/>
+      <c r="Z73" s="9"/>
+      <c r="AA73" s="9"/>
+      <c r="AB73" s="9"/>
+      <c r="AC73" s="9"/>
+      <c r="AD73" s="9"/>
+      <c r="AE73" s="9"/>
     </row>
     <row r="74" spans="3:31" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="K74" s="7" t="s">
+      <c r="K74" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="L74" s="7"/>
-      <c r="M74" s="7"/>
-      <c r="N74" s="7"/>
-      <c r="O74" s="7"/>
-      <c r="P74" s="7"/>
-      <c r="Q74" s="7"/>
+      <c r="L74" s="9"/>
+      <c r="M74" s="9"/>
+      <c r="N74" s="9"/>
+      <c r="O74" s="9"/>
+      <c r="P74" s="9"/>
+      <c r="Q74" s="9"/>
     </row>
     <row r="75" spans="3:31" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="K75" s="7" t="s">
+      <c r="K75" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="L75" s="7"/>
-      <c r="M75" s="7"/>
-      <c r="N75" s="7"/>
-      <c r="O75" s="7"/>
-      <c r="P75" s="7"/>
-      <c r="Q75" s="7"/>
+      <c r="L75" s="9"/>
+      <c r="M75" s="9"/>
+      <c r="N75" s="9"/>
+      <c r="O75" s="9"/>
+      <c r="P75" s="9"/>
+      <c r="Q75" s="9"/>
     </row>
     <row r="77" spans="3:31" x14ac:dyDescent="0.25">
       <c r="K77" t="s">
@@ -24878,11 +24897,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="L35:Q36"/>
-    <mergeCell ref="C35:E36"/>
-    <mergeCell ref="F35:K35"/>
-    <mergeCell ref="F36:K36"/>
-    <mergeCell ref="K72:Q72"/>
     <mergeCell ref="Y72:AE72"/>
     <mergeCell ref="Y73:AE73"/>
     <mergeCell ref="K74:Q74"/>
@@ -24890,6 +24904,11 @@
     <mergeCell ref="C72:E73"/>
     <mergeCell ref="R72:X73"/>
     <mergeCell ref="K73:Q73"/>
+    <mergeCell ref="L35:Q36"/>
+    <mergeCell ref="C35:E36"/>
+    <mergeCell ref="F35:K35"/>
+    <mergeCell ref="F36:K36"/>
+    <mergeCell ref="K72:Q72"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -24914,166 +24933,383 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C23"/>
+  <dimension ref="B2:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="50.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B2" s="15" t="s">
+    <row r="2" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B2" s="7" t="s">
         <v>21</v>
       </c>
+      <c r="D2" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="18" t="s">
         <v>18</v>
       </c>
+      <c r="C4" s="18" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="15" t="s">
         <v>22</v>
       </c>
+      <c r="D5" s="16">
+        <v>200</v>
+      </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="14" t="s">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="16">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" s="15" t="s">
         <v>23</v>
       </c>
+      <c r="D7" s="16">
+        <v>201</v>
+      </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="14" t="s">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="17"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="16">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C9" s="15" t="s">
         <v>25</v>
       </c>
+      <c r="D9" s="16">
+        <v>201</v>
+      </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="14" t="s">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="17"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="16">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="17"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="16">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="6"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="16">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="16">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="16">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="16">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="16">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="16">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="19" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="13" t="s">
-        <v>27</v>
+      <c r="C21" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="16">
+        <v>200</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" t="s">
-        <v>30</v>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="16">
+        <v>404</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>29</v>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="19" t="s">
+        <v>33</v>
       </c>
-      <c r="C12" t="s">
-        <v>31</v>
+      <c r="C23" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="16">
+        <v>201</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" t="s">
-        <v>42</v>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="16">
+        <v>400</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>26</v>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="19" t="s">
+        <v>34</v>
       </c>
-      <c r="C14" t="s">
-        <v>43</v>
+      <c r="C25" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" s="16">
+        <v>201</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" t="s">
-        <v>44</v>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="16">
+        <v>400</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>34</v>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="19" t="s">
+        <v>35</v>
       </c>
-      <c r="C16" t="s">
-        <v>45</v>
+      <c r="C27" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="16">
+        <v>200</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" t="s">
-        <v>46</v>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="16">
+        <v>404</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C29" s="19" t="s">
         <v>47</v>
       </c>
+      <c r="D29" s="16">
+        <v>201</v>
+      </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="16">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C31" s="19" t="s">
         <v>48</v>
       </c>
+      <c r="D31" s="16">
+        <v>201</v>
+      </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="16">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C33" s="19" t="s">
         <v>49</v>
       </c>
+      <c r="D33" s="16">
+        <v>200</v>
+      </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="16">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C35" s="19" t="s">
         <v>50</v>
       </c>
+      <c r="D35" s="16">
+        <v>200</v>
+      </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="16">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C37" s="19" t="s">
         <v>51</v>
       </c>
+      <c r="D37" s="16">
+        <v>200</v>
+      </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="16">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C39" s="19" t="s">
         <v>52</v>
+      </c>
+      <c r="D39" s="16">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="16">
+        <v>400</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="32">
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B5:B6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>